<commit_message>
_09_Soru  ve TODO 1 ve TODO 2
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/Carpim.xlsx
+++ b/src/test/java/ApachePOI/resource/Carpim.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TechnoStudy\IdeaProjects\Cucumber7\src\test\java\ApachePOI\resource\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,11 +24,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="2">
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -340,12 +348,353 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>